<commit_message>
pseudo MI e pseudo UC
</commit_message>
<xml_diff>
--- a/Definição_ISA.xlsx
+++ b/Definição_ISA.xlsx
@@ -11,18 +11,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
-  <si>
-    <t>20-23</t>
-  </si>
-  <si>
-    <t>15-19</t>
-  </si>
-  <si>
-    <t>10-14</t>
-  </si>
-  <si>
-    <t>0-4</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+  <si>
+    <t>21-23</t>
+  </si>
+  <si>
+    <t>16-20</t>
+  </si>
+  <si>
+    <t>11-15</t>
+  </si>
+  <si>
+    <t>0-2</t>
   </si>
   <si>
     <t>R</t>
@@ -37,13 +37,16 @@
     <t>RD</t>
   </si>
   <si>
+    <t>FUNC3</t>
+  </si>
+  <si>
     <t>OPCODE</t>
   </si>
   <si>
     <t>ADD, SUB, MUL, DIV, SLL, SLT</t>
   </si>
   <si>
-    <t>15-23</t>
+    <t>16-23</t>
   </si>
   <si>
     <t>I</t>
@@ -53,6 +56,12 @@
   </si>
   <si>
     <t>ADDI, SLLI, SLTI, LW, JALR</t>
+  </si>
+  <si>
+    <t>18-23</t>
+  </si>
+  <si>
+    <t>13-17</t>
   </si>
   <si>
     <t>S</t>
@@ -424,7 +433,10 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="23.25"/>
-    <col customWidth="1" min="6" max="6" width="21.38"/>
+    <col customWidth="1" min="6" max="6" width="12.75"/>
+    <col customWidth="1" min="8" max="8" width="12.13"/>
+    <col customWidth="1" min="9" max="9" width="10.75"/>
+    <col customWidth="1" min="10" max="10" width="8.88"/>
     <col customWidth="1" min="11" max="11" width="52.88"/>
   </cols>
   <sheetData>
@@ -432,17 +444,20 @@
       <c r="E6" s="1"/>
     </row>
     <row r="7">
+      <c r="E7" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="F7" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="H7" s="3">
+        <v>45571.0</v>
+      </c>
       <c r="I7" s="3">
-        <v>45540.0</v>
+        <v>45415.0</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>3</v>
@@ -450,41 +465,48 @@
       <c r="K7" s="4"/>
     </row>
     <row r="8">
-      <c r="E8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="G8" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
-      <c r="E9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="I9" s="4"/>
       <c r="K9" s="4"/>
     </row>
     <row r="10">
-      <c r="E10" s="4"/>
-      <c r="F10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="2" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="H10" s="3">
+        <v>45571.0</v>
+      </c>
       <c r="I10" s="3">
-        <v>45540.0</v>
+        <v>45415.0</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>3</v>
@@ -492,43 +514,48 @@
       <c r="K10" s="4"/>
     </row>
     <row r="11">
-      <c r="E11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="9" t="s">
+      <c r="D11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="10"/>
+      <c r="E11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="H11" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12">
-      <c r="E12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="I12" s="4"/>
       <c r="K12" s="4"/>
     </row>
     <row r="13">
-      <c r="E13" s="4"/>
-      <c r="F13" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="8"/>
       <c r="G13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="H13" s="3">
+        <v>45634.0</v>
       </c>
       <c r="I13" s="3">
-        <v>45540.0</v>
+        <v>45476.0</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>3</v>
@@ -536,12 +563,13 @@
       <c r="K13" s="4"/>
     </row>
     <row r="14">
-      <c r="E14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="D14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="10"/>
       <c r="G14" s="6" t="s">
         <v>5</v>
       </c>
@@ -549,30 +577,34 @@
         <v>6</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15">
-      <c r="E15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="I15" s="4"/>
       <c r="K15" s="4"/>
     </row>
     <row r="16">
-      <c r="E16" s="4"/>
-      <c r="F16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="2" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="H16" s="3">
+        <v>45571.0</v>
+      </c>
       <c r="I16" s="3">
-        <v>45540.0</v>
+        <v>45415.0</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>3</v>
@@ -580,39 +612,44 @@
       <c r="K16" s="4"/>
     </row>
     <row r="17">
-      <c r="E17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="10"/>
+      <c r="D17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="H17" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18">
-      <c r="E18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="I18" s="4"/>
       <c r="K18" s="4"/>
     </row>
     <row r="19">
-      <c r="E19" s="4"/>
-      <c r="F19" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="8"/>
       <c r="I19" s="3">
-        <v>45540.0</v>
+        <v>45476.0</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>3</v>
@@ -620,32 +657,35 @@
       <c r="K19" s="4"/>
     </row>
     <row r="20">
-      <c r="E20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="D20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="12"/>
       <c r="G20" s="12"/>
       <c r="H20" s="10"/>
       <c r="I20" s="6" t="s">
         <v>7</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F19:H19"/>
+  <mergeCells count="8">
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E13:F13"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Arrumar UC e ver proc.IMM
</commit_message>
<xml_diff>
--- a/Definição_ISA.xlsx
+++ b/Definição_ISA.xlsx
@@ -11,15 +11,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
-  <si>
-    <t>21-23</t>
-  </si>
-  <si>
-    <t>16-20</t>
-  </si>
-  <si>
-    <t>11-15</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
+  <si>
+    <t>18-23</t>
+  </si>
+  <si>
+    <t>14-17</t>
+  </si>
+  <si>
+    <t>10-13</t>
   </si>
   <si>
     <t>0-2</t>
@@ -46,7 +46,7 @@
     <t>ADD, SUB, MUL, DIV, SLL, SLT</t>
   </si>
   <si>
-    <t>16-23</t>
+    <t>14-23</t>
   </si>
   <si>
     <t>I</t>
@@ -58,12 +58,6 @@
     <t>ADDI, SLLI, SLTI, LW, JALR</t>
   </si>
   <si>
-    <t>18-23</t>
-  </si>
-  <si>
-    <t>13-17</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -76,7 +70,7 @@
     <t>BEQ, BNE, BLT, BGE</t>
   </si>
   <si>
-    <t>10-23</t>
+    <t>7-23</t>
   </si>
   <si>
     <t>J</t>
@@ -454,7 +448,7 @@
         <v>2</v>
       </c>
       <c r="H7" s="3">
-        <v>45571.0</v>
+        <v>45541.0</v>
       </c>
       <c r="I7" s="3">
         <v>45415.0</v>
@@ -503,7 +497,7 @@
         <v>2</v>
       </c>
       <c r="H10" s="3">
-        <v>45571.0</v>
+        <v>45541.0</v>
       </c>
       <c r="I10" s="3">
         <v>45415.0</v>
@@ -545,17 +539,17 @@
     <row r="13">
       <c r="D13" s="4"/>
       <c r="E13" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="2" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="H13" s="3">
-        <v>45634.0</v>
+        <v>45572.0</v>
       </c>
       <c r="I13" s="3">
-        <v>45476.0</v>
+        <v>45446.0</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>3</v>
@@ -564,7 +558,7 @@
     </row>
     <row r="14">
       <c r="D14" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>13</v>
@@ -583,7 +577,7 @@
         <v>9</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15">
@@ -601,7 +595,7 @@
         <v>2</v>
       </c>
       <c r="H16" s="3">
-        <v>45571.0</v>
+        <v>45541.0</v>
       </c>
       <c r="I16" s="3">
         <v>45415.0</v>
@@ -613,7 +607,7 @@
     </row>
     <row r="17">
       <c r="D17" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>13</v>
@@ -632,7 +626,7 @@
         <v>9</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18">
@@ -643,13 +637,13 @@
     <row r="19">
       <c r="D19" s="4"/>
       <c r="E19" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="8"/>
       <c r="I19" s="3">
-        <v>45476.0</v>
+        <v>45446.0</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>3</v>
@@ -658,7 +652,7 @@
     </row>
     <row r="20">
       <c r="D20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>13</v>
@@ -673,7 +667,7 @@
         <v>9</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pseudo proc; falta jal e jalr
</commit_message>
<xml_diff>
--- a/Definição_ISA.xlsx
+++ b/Definição_ISA.xlsx
@@ -344,40 +344,44 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -572,345 +576,345 @@
   </sheetPr>
   <dimension ref="D6:L36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I31" activeCellId="0" sqref="I31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K29" activeCellId="0" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="52.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="52.88"/>
   </cols>
   <sheetData>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E6" s="1"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="3" t="n">
+      <c r="H7" s="4" t="n">
         <v>45541</v>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="I7" s="4" t="n">
         <v>45415</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="1"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="1"/>
-      <c r="E10" s="2" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="3" t="n">
+      <c r="H10" s="4" t="n">
         <v>45541</v>
       </c>
-      <c r="I10" s="3" t="n">
+      <c r="I10" s="4" t="n">
         <v>45415</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K10" s="1"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4" t="s">
+      <c r="F11" s="5"/>
+      <c r="G11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="1"/>
-      <c r="E13" s="2" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
+      <c r="F13" s="3"/>
+      <c r="G13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="3" t="n">
+      <c r="H13" s="4" t="n">
         <v>45541</v>
       </c>
-      <c r="I13" s="3" t="n">
+      <c r="I13" s="4" t="n">
         <v>45415</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K13" s="1"/>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4" t="s">
+      <c r="F14" s="5"/>
+      <c r="G14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K14" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="1"/>
-      <c r="E16" s="2" t="s">
+      <c r="D16" s="2"/>
+      <c r="E16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="5" t="n">
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="6" t="n">
         <v>45541</v>
       </c>
-      <c r="I16" s="3" t="n">
+      <c r="I16" s="4" t="n">
         <v>45415</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K16" s="1"/>
+      <c r="K16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="6" t="s">
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L17" s="7"/>
+      <c r="L17" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D36" s="8" t="s">
+    <row r="36" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D36" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="9" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
opcode e func3 ?
</commit_message>
<xml_diff>
--- a/Definição_ISA.xlsx
+++ b/Definição_ISA.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Página1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Página1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +22,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>Autor desconhecido</author>
   </authors>
   <commentList>
     <comment ref="D8" authorId="0">
@@ -30,10 +30,8 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">ADD: XXXXXXXXXXXXXXXXXX000 000
 SUB:
@@ -54,10 +52,8 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">ADDI: XXXXXXXXXXXXXXXXXX000001
 SLLI:
@@ -76,10 +72,8 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">SW: XXXXXXXXXXXXXXXXXX000010
 BEQ:
@@ -98,10 +92,8 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">JAL: XXXXXXXXXXXXXXXXXX000011</t>
         </r>
@@ -112,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
   <si>
     <t xml:space="preserve">18-23</t>
   </si>
@@ -126,6 +118,9 @@
     <t xml:space="preserve">0-2</t>
   </si>
   <si>
+    <t xml:space="preserve">OPCODE</t>
+  </si>
+  <si>
     <t xml:space="preserve">R</t>
   </si>
   <si>
@@ -141,12 +136,12 @@
     <t xml:space="preserve">FUNC3</t>
   </si>
   <si>
-    <t xml:space="preserve">OPCODE</t>
-  </si>
-  <si>
     <t xml:space="preserve">ADD, SUB, MUL, DIV, SLL, SLT</t>
   </si>
   <si>
+    <t xml:space="preserve">0.0.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">14-23</t>
   </si>
   <si>
@@ -159,12 +154,18 @@
     <t xml:space="preserve">ADDI, SLLI, SLTI, LW, JALR</t>
   </si>
   <si>
+    <t xml:space="preserve">0.0.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">S &amp; B</t>
   </si>
   <si>
     <t xml:space="preserve">SW, BEQ, BNE, BLT, BGE</t>
   </si>
   <si>
+    <t xml:space="preserve">0.1.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">10-23</t>
   </si>
   <si>
@@ -174,6 +175,9 @@
     <t xml:space="preserve">JAL</t>
   </si>
   <si>
+    <t xml:space="preserve">0.1.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">ADD</t>
   </si>
   <si>
@@ -183,6 +187,9 @@
     <t xml:space="preserve">RD ← RS1 + RS2</t>
   </si>
   <si>
+    <t xml:space="preserve">WHICH_R; WR; MU_PC</t>
+  </si>
+  <si>
     <t xml:space="preserve">SUB</t>
   </si>
   <si>
@@ -219,12 +226,36 @@
     <t xml:space="preserve">RD ← RS1 + IMM</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">WR; MU_IMM; MU_ULA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">; MU_PC</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">SLLI</t>
   </si>
   <si>
     <t xml:space="preserve">RD ← RS1 « IMM</t>
   </si>
   <si>
+    <t xml:space="preserve">WR; MU_IMM; MU_ULA; MU_PC</t>
+  </si>
+  <si>
     <t xml:space="preserve">SLTI</t>
   </si>
   <si>
@@ -237,12 +268,18 @@
     <t xml:space="preserve">RD ← MD[RS1 + IMM]</t>
   </si>
   <si>
+    <t xml:space="preserve">WR; MU_IMM; MU_ULA; MR; MU_PC</t>
+  </si>
+  <si>
     <t xml:space="preserve">SW</t>
   </si>
   <si>
     <t xml:space="preserve">MD[RS1 + IMM] ← RS2</t>
   </si>
   <si>
+    <t xml:space="preserve">WHICH_R; WR; MU_IMM; MU_ULA; WM; MU_PC</t>
+  </si>
+  <si>
     <t xml:space="preserve">BEQ</t>
   </si>
   <si>
@@ -252,12 +289,36 @@
     <t xml:space="preserve">(RS1 == RS2) ? PC+=IMM : PC+=4</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">WHICH_R; OP_B; IS_BRANCH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">; MU_PC</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">BNE</t>
   </si>
   <si>
     <t xml:space="preserve">(RS1 != RS2) ? PC+=IMM : PC+=4</t>
   </si>
   <si>
+    <t xml:space="preserve">WHICH_R; OP_B; IS_BRANCH; MU_PC</t>
+  </si>
+  <si>
     <t xml:space="preserve">BLT</t>
   </si>
   <si>
@@ -274,6 +335,27 @@
   </si>
   <si>
     <t xml:space="preserve">RD ← PC+4</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">WR; MU_IMM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">; MU_PC</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">JALR</t>
@@ -286,12 +368,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d\-m"/>
-    <numFmt numFmtId="166" formatCode="yyyy\.m\.d"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -322,10 +403,15 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -398,7 +484,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -419,14 +505,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -435,24 +521,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -467,15 +545,121 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="D6:L36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -486,7 +670,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="52.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="25.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="25.56"/>
   </cols>
   <sheetData>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -512,41 +696,47 @@
         <v>3</v>
       </c>
       <c r="K7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L7" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="6"/>
+      <c r="L8" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="2"/>
       <c r="I9" s="2"/>
       <c r="K9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="2"/>
       <c r="E10" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
@@ -562,41 +752,45 @@
         <v>3</v>
       </c>
       <c r="K10" s="2"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="5" t="s">
+      <c r="E11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="H11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="I11" s="6" t="s">
         <v>9</v>
       </c>
+      <c r="J11" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="K11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="2"/>
       <c r="I12" s="2"/>
       <c r="K12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="2"/>
       <c r="E13" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
@@ -612,41 +806,45 @@
         <v>3</v>
       </c>
       <c r="K13" s="2"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J14" s="5" t="s">
+      <c r="I14" s="6" t="s">
         <v>9</v>
       </c>
+      <c r="J14" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="K14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L14" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="2"/>
       <c r="I15" s="2"/>
       <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="2"/>
       <c r="E16" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -660,215 +858,269 @@
         <v>3</v>
       </c>
       <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
       <c r="H17" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L17" s="9"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="10" t="s">
+      <c r="L17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="11" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D20" s="9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="11" t="s">
+      <c r="F20" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="10" t="s">
+      <c r="K20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" s="11" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="10" t="s">
+      <c r="E21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" s="11" t="s">
+      <c r="K21" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="10" t="s">
+      <c r="E22" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" s="11" t="s">
+      <c r="K22" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D23" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="10" t="s">
+      <c r="E23" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" s="11" t="s">
+      <c r="K23" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="10" t="s">
+      <c r="E24" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27" s="11" t="s">
+      <c r="K24" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="10" t="s">
+      <c r="E25" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F28" s="11" t="s">
+      <c r="K25" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D26" s="9" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="10" t="s">
+      <c r="E26" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" s="11" t="s">
+      <c r="K26" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="10" t="s">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D27" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F30" s="11" t="s">
+      <c r="E27" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="10" t="s">
+      <c r="K27" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="10" t="s">
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D28" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="E28" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="10" t="s">
+      <c r="K28" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D29" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F32" s="11" t="s">
+      <c r="E29" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="10" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="10" t="s">
+      <c r="K29" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E33" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F33" s="11" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D30" s="9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="10" t="s">
+      <c r="E30" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" s="11" t="s">
+      <c r="K30" s="11" t="s">
         <v>51</v>
       </c>
     </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D31" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D32" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="K32" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D33" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="K33" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D34" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="35" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>53</v>
+      <c r="D35" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>53</v>
+      <c r="D36" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fazer assembly para testar
</commit_message>
<xml_diff>
--- a/Definição_ISA.xlsx
+++ b/Definição_ISA.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Página1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Página1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +22,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>Autor desconhecido</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="D8" authorId="0">
@@ -30,8 +30,10 @@
         <r>
           <rPr>
             <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">ADD: XXXXXXXXXXXXXXXXXX000 000
 SUB:
@@ -52,8 +54,10 @@
         <r>
           <rPr>
             <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">ADDI: XXXXXXXXXXXXXXXXXX000001
 SLLI:
@@ -72,8 +76,10 @@
         <r>
           <rPr>
             <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">SW: XXXXXXXXXXXXXXXXXX000010
 BEQ:
@@ -92,8 +98,10 @@
         <r>
           <rPr>
             <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">JAL: XXXXXXXXXXXXXXXXXX000011</t>
         </r>
@@ -104,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="62">
   <si>
     <t xml:space="preserve">18-23</t>
   </si>
@@ -118,30 +126,27 @@
     <t xml:space="preserve">0-2</t>
   </si>
   <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNC3</t>
+  </si>
+  <si>
     <t xml:space="preserve">OPCODE</t>
   </si>
   <si>
-    <t xml:space="preserve">R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNC3</t>
-  </si>
-  <si>
     <t xml:space="preserve">ADD, SUB, MUL, DIV, SLL, SLT</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">14-23</t>
   </si>
   <si>
@@ -154,18 +159,12 @@
     <t xml:space="preserve">ADDI, SLLI, SLTI, LW, JALR</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">S &amp; B</t>
   </si>
   <si>
     <t xml:space="preserve">SW, BEQ, BNE, BLT, BGE</t>
   </si>
   <si>
-    <t xml:space="preserve">0.1.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">10-23</t>
   </si>
   <si>
@@ -175,9 +174,6 @@
     <t xml:space="preserve">JAL</t>
   </si>
   <si>
-    <t xml:space="preserve">0.1.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">ADD</t>
   </si>
   <si>
@@ -187,7 +183,7 @@
     <t xml:space="preserve">RD ← RS1 + RS2</t>
   </si>
   <si>
-    <t xml:space="preserve">WHICH_R; WR; MU_PC</t>
+    <t xml:space="preserve">WR</t>
   </si>
   <si>
     <t xml:space="preserve">SUB</t>
@@ -226,25 +222,7 @@
     <t xml:space="preserve">RD ← RS1 + IMM</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">WR; MU_IMM; MU_ULA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">; MU_PC</t>
-    </r>
+    <t xml:space="preserve">WR; MU_IMM; MU_ULA; MU_PC</t>
   </si>
   <si>
     <t xml:space="preserve">SLLI</t>
@@ -253,9 +231,6 @@
     <t xml:space="preserve">RD ← RS1 « IMM</t>
   </si>
   <si>
-    <t xml:space="preserve">WR; MU_IMM; MU_ULA; MU_PC</t>
-  </si>
-  <si>
     <t xml:space="preserve">SLTI</t>
   </si>
   <si>
@@ -268,7 +243,7 @@
     <t xml:space="preserve">RD ← MD[RS1 + IMM]</t>
   </si>
   <si>
-    <t xml:space="preserve">WR; MU_IMM; MU_ULA; MR; MU_PC</t>
+    <t xml:space="preserve">WR; MU_IMM; MU_ULA; MR</t>
   </si>
   <si>
     <t xml:space="preserve">SW</t>
@@ -277,7 +252,7 @@
     <t xml:space="preserve">MD[RS1 + IMM] ← RS2</t>
   </si>
   <si>
-    <t xml:space="preserve">WHICH_R; WR; MU_IMM; MU_ULA; WM; MU_PC</t>
+    <t xml:space="preserve">WHICH_R; WR; MU_IMM; MU_ULA; WM</t>
   </si>
   <si>
     <t xml:space="preserve">BEQ</t>
@@ -289,25 +264,7 @@
     <t xml:space="preserve">(RS1 == RS2) ? PC+=IMM : PC+=4</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">WHICH_R; OP_B; IS_BRANCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">; MU_PC</t>
-    </r>
+    <t xml:space="preserve">WHICH_R; OP_B; IS_BRANCH; MU_PC</t>
   </si>
   <si>
     <t xml:space="preserve">BNE</t>
@@ -316,9 +273,6 @@
     <t xml:space="preserve">(RS1 != RS2) ? PC+=IMM : PC+=4</t>
   </si>
   <si>
-    <t xml:space="preserve">WHICH_R; OP_B; IS_BRANCH; MU_PC</t>
-  </si>
-  <si>
     <t xml:space="preserve">BLT</t>
   </si>
   <si>
@@ -337,25 +291,7 @@
     <t xml:space="preserve">RD ← PC+4</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">WR; MU_IMM</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">; MU_PC</t>
-    </r>
+    <t xml:space="preserve">WR; MU_ULA; MU_PC</t>
   </si>
   <si>
     <t xml:space="preserve">JALR</t>
@@ -372,7 +308,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d\-m"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -401,17 +337,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -529,7 +454,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -545,129 +470,23 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="D6:L36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J28" activeCellId="0" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="52.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="25.56"/>
@@ -696,36 +515,32 @@
         <v>3</v>
       </c>
       <c r="K7" s="2"/>
-      <c r="L7" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="L7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="J8" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>4</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="L8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="2"/>
@@ -736,7 +551,7 @@
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="2"/>
       <c r="E10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
@@ -756,30 +571,28 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="I11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="J11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>4</v>
-      </c>
       <c r="K11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="L11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="2"/>
@@ -790,7 +603,7 @@
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="2"/>
       <c r="E13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
@@ -810,30 +623,28 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="6" t="s">
-        <v>4</v>
-      </c>
       <c r="K14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="L14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="2"/>
@@ -844,7 +655,7 @@
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="2"/>
       <c r="E16" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -862,265 +673,263 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="L17" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E21" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="K21" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="E22" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="9" t="s">
+      <c r="K22" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D23" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="10" t="s">
+      <c r="E23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="K21" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="9" t="s">
+      <c r="K23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="10" t="s">
+      <c r="E24" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K22" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="9" t="s">
+      <c r="K24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="10" t="s">
+      <c r="E25" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="K23" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="K25" s="11" t="s">
-        <v>27</v>
+      <c r="K25" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D27" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D29" s="9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K29" s="11" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="K30" s="11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D31" s="9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D32" s="9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="K32" s="11" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="9" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="K33" s="11" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D34" s="9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="K34" s="11" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D35" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D36" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
teste media deu certo
</commit_message>
<xml_diff>
--- a/Definição_ISA.xlsx
+++ b/Definição_ISA.xlsx
@@ -495,11 +495,11 @@
   </sheetPr>
   <dimension ref="D6:L36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I35" activeCellId="0" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.75"/>

</xml_diff>